<commit_message>
rapport fct 3 et fct 5
</commit_message>
<xml_diff>
--- a/fonctions3et5.xlsx
+++ b/fonctions3et5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\heig-vd\BA2\ASD1\labos\labo01\ASD1_LABO1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B58AAF-5DF9-4026-BEF2-71211C00AC15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1CD708-EDAA-416F-B3F3-E4741F6D8792}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1728" yWindow="1476" windowWidth="17280" windowHeight="8964" xr2:uid="{CAEF022A-5CEE-4E9B-B41F-DD89C75AB3A7}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{CAEF022A-5CEE-4E9B-B41F-DD89C75AB3A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023BE48E-74C9-48D0-B02A-B5E9D9ABC198}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>